<commit_message>
Added more articles to be imported
</commit_message>
<xml_diff>
--- a/products/fixtures/articles.xlsx
+++ b/products/fixtures/articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djang\Documents\Soccersystems\products\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC677C4-8EDD-4D37-A4E8-3955508C59CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD070F5-5CAA-4DB9-9B02-7370F569AA64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="379">
   <si>
     <t>id</t>
   </si>
@@ -769,9 +769,6 @@
     <t>Naamblok KUDUS</t>
   </si>
   <si>
-    <t>serial</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -797,6 +794,369 @@
   </si>
   <si>
     <t>item_group</t>
+  </si>
+  <si>
+    <t>XA202500</t>
+  </si>
+  <si>
+    <t>XA202501</t>
+  </si>
+  <si>
+    <t>XA202502</t>
+  </si>
+  <si>
+    <t>XA202503</t>
+  </si>
+  <si>
+    <t>XA202504</t>
+  </si>
+  <si>
+    <t>XA202505</t>
+  </si>
+  <si>
+    <t>XA202506</t>
+  </si>
+  <si>
+    <t>XA202507</t>
+  </si>
+  <si>
+    <t>XA202508</t>
+  </si>
+  <si>
+    <t>XA202509</t>
+  </si>
+  <si>
+    <t>XA201600</t>
+  </si>
+  <si>
+    <t>XA201601</t>
+  </si>
+  <si>
+    <t>XA201602</t>
+  </si>
+  <si>
+    <t>XA201603</t>
+  </si>
+  <si>
+    <t>XA201604</t>
+  </si>
+  <si>
+    <t>XA201605</t>
+  </si>
+  <si>
+    <t>XA201606</t>
+  </si>
+  <si>
+    <t>XA201607</t>
+  </si>
+  <si>
+    <t>XA201608</t>
+  </si>
+  <si>
+    <t>XA201609</t>
+  </si>
+  <si>
+    <t>XA201000</t>
+  </si>
+  <si>
+    <t>XA201001</t>
+  </si>
+  <si>
+    <t>XA201002</t>
+  </si>
+  <si>
+    <t>XA201003</t>
+  </si>
+  <si>
+    <t>XA201004</t>
+  </si>
+  <si>
+    <t>XA201005</t>
+  </si>
+  <si>
+    <t>XA201006</t>
+  </si>
+  <si>
+    <t>XA201007</t>
+  </si>
+  <si>
+    <t>XA201008</t>
+  </si>
+  <si>
+    <t>XA201009</t>
+  </si>
+  <si>
+    <t>XA20060A</t>
+  </si>
+  <si>
+    <t>XA20060B</t>
+  </si>
+  <si>
+    <t>XA20060C</t>
+  </si>
+  <si>
+    <t>XA20060D</t>
+  </si>
+  <si>
+    <t>XA20060E</t>
+  </si>
+  <si>
+    <t>XA20060F</t>
+  </si>
+  <si>
+    <t>XA20060G</t>
+  </si>
+  <si>
+    <t>XA20060H</t>
+  </si>
+  <si>
+    <t>XA20060I</t>
+  </si>
+  <si>
+    <t>XA20060J</t>
+  </si>
+  <si>
+    <t>XA20060K</t>
+  </si>
+  <si>
+    <t>XA20060L</t>
+  </si>
+  <si>
+    <t>XA20060M</t>
+  </si>
+  <si>
+    <t>XA20060N</t>
+  </si>
+  <si>
+    <t>XA20060O</t>
+  </si>
+  <si>
+    <t>XA20060P</t>
+  </si>
+  <si>
+    <t>XA20060Q</t>
+  </si>
+  <si>
+    <t>XA20060R</t>
+  </si>
+  <si>
+    <t>XA20060S</t>
+  </si>
+  <si>
+    <t>XA20060T</t>
+  </si>
+  <si>
+    <t>XA20060U</t>
+  </si>
+  <si>
+    <t>XA20060V</t>
+  </si>
+  <si>
+    <t>XA20060W</t>
+  </si>
+  <si>
+    <t>XA20060X</t>
+  </si>
+  <si>
+    <t>XA20060Y</t>
+  </si>
+  <si>
+    <t>XA20060Z</t>
+  </si>
+  <si>
+    <t>XA20060_</t>
+  </si>
+  <si>
+    <t>XA200600</t>
+  </si>
+  <si>
+    <t>XA2006AZ</t>
+  </si>
+  <si>
+    <t>XA2006AY</t>
+  </si>
+  <si>
+    <t>XA2006BL</t>
+  </si>
+  <si>
+    <t>XA2006BD</t>
+  </si>
+  <si>
+    <t>XA2006BN</t>
+  </si>
+  <si>
+    <t>XA2006DO</t>
+  </si>
+  <si>
+    <t>XA2006DW</t>
+  </si>
+  <si>
+    <t>XA2006DS</t>
+  </si>
+  <si>
+    <t>XA2006EG</t>
+  </si>
+  <si>
+    <t>XA2006EP</t>
+  </si>
+  <si>
+    <t>XA2006GH</t>
+  </si>
+  <si>
+    <t>XA2006HN</t>
+  </si>
+  <si>
+    <t>XA2006HR</t>
+  </si>
+  <si>
+    <t>XA2006JR</t>
+  </si>
+  <si>
+    <t>XA2006KN</t>
+  </si>
+  <si>
+    <t>XA2006KR</t>
+  </si>
+  <si>
+    <t>XA2006KS</t>
+  </si>
+  <si>
+    <t>XA2006LD</t>
+  </si>
+  <si>
+    <t>XA2006LG</t>
+  </si>
+  <si>
+    <t>XA2006MN</t>
+  </si>
+  <si>
+    <t>XA2006MZ</t>
+  </si>
+  <si>
+    <t>XA2006MI</t>
+  </si>
+  <si>
+    <t>XA2006NS</t>
+  </si>
+  <si>
+    <t>XA2006PE</t>
+  </si>
+  <si>
+    <t>XA2006PS</t>
+  </si>
+  <si>
+    <t>XA2006QR</t>
+  </si>
+  <si>
+    <t>XA2006SS</t>
+  </si>
+  <si>
+    <t>XA2006TC</t>
+  </si>
+  <si>
+    <t>XA2006TO</t>
+  </si>
+  <si>
+    <t>XA2006TR</t>
+  </si>
+  <si>
+    <t>XA2006TE</t>
+  </si>
+  <si>
+    <t>XA2006UR</t>
+  </si>
+  <si>
+    <t>XA2006VK</t>
+  </si>
+  <si>
+    <t>XA2006ZH</t>
+  </si>
+  <si>
+    <t>XA20040A</t>
+  </si>
+  <si>
+    <t>XA20040B</t>
+  </si>
+  <si>
+    <t>XA20040C</t>
+  </si>
+  <si>
+    <t>XA20040D</t>
+  </si>
+  <si>
+    <t>XA20040E</t>
+  </si>
+  <si>
+    <t>XA20040F</t>
+  </si>
+  <si>
+    <t>XA20040G</t>
+  </si>
+  <si>
+    <t>XA20040H</t>
+  </si>
+  <si>
+    <t>XA20040I</t>
+  </si>
+  <si>
+    <t>XA20040J</t>
+  </si>
+  <si>
+    <t>XA20040K</t>
+  </si>
+  <si>
+    <t>XA20040L</t>
+  </si>
+  <si>
+    <t>XA20040M</t>
+  </si>
+  <si>
+    <t>XA20040N</t>
+  </si>
+  <si>
+    <t>XA20040O</t>
+  </si>
+  <si>
+    <t>XA20040P</t>
+  </si>
+  <si>
+    <t>XA20040Q</t>
+  </si>
+  <si>
+    <t>XA20040R</t>
+  </si>
+  <si>
+    <t>XA20040S</t>
+  </si>
+  <si>
+    <t>XA20040T</t>
+  </si>
+  <si>
+    <t>XA20040U</t>
+  </si>
+  <si>
+    <t>XA20040V</t>
+  </si>
+  <si>
+    <t>XA20040W</t>
+  </si>
+  <si>
+    <t>XA20040X</t>
+  </si>
+  <si>
+    <t>XA20040Y</t>
+  </si>
+  <si>
+    <t>XA20040Z</t>
+  </si>
+  <si>
+    <t>XA200400</t>
+  </si>
+  <si>
+    <t>XA20040_</t>
+  </si>
+  <si>
+    <t>slug</t>
   </si>
 </sst>
 </file>
@@ -1167,10 +1527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H131"/>
+  <dimension ref="A1:H251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134:B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,22 +1548,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -2962,7 +3322,7 @@
         <v>2</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>188</v>
@@ -3352,10 +3712,10 @@
         <v>1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F84" s="4">
         <v>6</v>
@@ -3378,10 +3738,10 @@
         <v>1</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F85" s="4">
         <v>6</v>
@@ -4574,7 +4934,7 @@
         <v>2</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>246</v>
@@ -4586,6 +4946,3126 @@
         <v>0.13</v>
       </c>
       <c r="H131" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>131</v>
+      </c>
+      <c r="B132" s="2">
+        <v>3</v>
+      </c>
+      <c r="C132" s="2">
+        <v>3</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F132" s="4">
+        <v>25</v>
+      </c>
+      <c r="G132" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>132</v>
+      </c>
+      <c r="B133" s="2">
+        <v>3</v>
+      </c>
+      <c r="C133" s="2">
+        <v>3</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F133" s="4">
+        <v>25</v>
+      </c>
+      <c r="G133" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>133</v>
+      </c>
+      <c r="B134" s="2">
+        <v>3</v>
+      </c>
+      <c r="C134" s="2">
+        <v>3</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F134" s="4">
+        <v>25</v>
+      </c>
+      <c r="G134" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>134</v>
+      </c>
+      <c r="B135" s="2">
+        <v>3</v>
+      </c>
+      <c r="C135" s="2">
+        <v>3</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F135" s="4">
+        <v>25</v>
+      </c>
+      <c r="G135" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>135</v>
+      </c>
+      <c r="B136" s="2">
+        <v>3</v>
+      </c>
+      <c r="C136" s="2">
+        <v>3</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F136" s="4">
+        <v>25</v>
+      </c>
+      <c r="G136" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>136</v>
+      </c>
+      <c r="B137" s="2">
+        <v>3</v>
+      </c>
+      <c r="C137" s="2">
+        <v>3</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F137" s="4">
+        <v>25</v>
+      </c>
+      <c r="G137" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>137</v>
+      </c>
+      <c r="B138" s="2">
+        <v>3</v>
+      </c>
+      <c r="C138" s="2">
+        <v>3</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F138" s="4">
+        <v>25</v>
+      </c>
+      <c r="G138" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>138</v>
+      </c>
+      <c r="B139" s="2">
+        <v>3</v>
+      </c>
+      <c r="C139" s="2">
+        <v>3</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F139" s="4">
+        <v>25</v>
+      </c>
+      <c r="G139" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>139</v>
+      </c>
+      <c r="B140" s="2">
+        <v>3</v>
+      </c>
+      <c r="C140" s="2">
+        <v>3</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F140" s="4">
+        <v>25</v>
+      </c>
+      <c r="G140" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>140</v>
+      </c>
+      <c r="B141" s="2">
+        <v>3</v>
+      </c>
+      <c r="C141" s="2">
+        <v>3</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F141" s="4">
+        <v>25</v>
+      </c>
+      <c r="G141" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>141</v>
+      </c>
+      <c r="B142" s="2">
+        <v>3</v>
+      </c>
+      <c r="C142" s="2">
+        <v>3</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F142" s="4">
+        <v>16</v>
+      </c>
+      <c r="G142" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>142</v>
+      </c>
+      <c r="B143" s="2">
+        <v>3</v>
+      </c>
+      <c r="C143" s="2">
+        <v>3</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F143" s="4">
+        <v>16</v>
+      </c>
+      <c r="G143" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>143</v>
+      </c>
+      <c r="B144" s="2">
+        <v>3</v>
+      </c>
+      <c r="C144" s="2">
+        <v>3</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F144" s="4">
+        <v>16</v>
+      </c>
+      <c r="G144" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>144</v>
+      </c>
+      <c r="B145" s="2">
+        <v>3</v>
+      </c>
+      <c r="C145" s="2">
+        <v>3</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F145" s="4">
+        <v>16</v>
+      </c>
+      <c r="G145" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>145</v>
+      </c>
+      <c r="B146" s="2">
+        <v>3</v>
+      </c>
+      <c r="C146" s="2">
+        <v>3</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F146" s="4">
+        <v>16</v>
+      </c>
+      <c r="G146" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H146" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>146</v>
+      </c>
+      <c r="B147" s="2">
+        <v>3</v>
+      </c>
+      <c r="C147" s="2">
+        <v>3</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F147" s="4">
+        <v>16</v>
+      </c>
+      <c r="G147" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>147</v>
+      </c>
+      <c r="B148" s="2">
+        <v>3</v>
+      </c>
+      <c r="C148" s="2">
+        <v>3</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F148" s="4">
+        <v>16</v>
+      </c>
+      <c r="G148" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>148</v>
+      </c>
+      <c r="B149" s="2">
+        <v>3</v>
+      </c>
+      <c r="C149" s="2">
+        <v>3</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F149" s="4">
+        <v>16</v>
+      </c>
+      <c r="G149" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>149</v>
+      </c>
+      <c r="B150" s="2">
+        <v>3</v>
+      </c>
+      <c r="C150" s="2">
+        <v>3</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F150" s="4">
+        <v>16</v>
+      </c>
+      <c r="G150" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H150" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>150</v>
+      </c>
+      <c r="B151" s="2">
+        <v>3</v>
+      </c>
+      <c r="C151" s="2">
+        <v>3</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F151" s="4">
+        <v>16</v>
+      </c>
+      <c r="G151" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>151</v>
+      </c>
+      <c r="B152" s="2">
+        <v>3</v>
+      </c>
+      <c r="C152" s="2">
+        <v>3</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F152" s="4">
+        <v>10</v>
+      </c>
+      <c r="G152" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>152</v>
+      </c>
+      <c r="B153" s="2">
+        <v>3</v>
+      </c>
+      <c r="C153" s="2">
+        <v>3</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F153" s="4">
+        <v>10</v>
+      </c>
+      <c r="G153" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H153" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>153</v>
+      </c>
+      <c r="B154" s="2">
+        <v>3</v>
+      </c>
+      <c r="C154" s="2">
+        <v>3</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F154" s="4">
+        <v>10</v>
+      </c>
+      <c r="G154" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>154</v>
+      </c>
+      <c r="B155" s="2">
+        <v>3</v>
+      </c>
+      <c r="C155" s="2">
+        <v>3</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F155" s="4">
+        <v>10</v>
+      </c>
+      <c r="G155" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H155" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>155</v>
+      </c>
+      <c r="B156" s="2">
+        <v>3</v>
+      </c>
+      <c r="C156" s="2">
+        <v>3</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F156" s="4">
+        <v>10</v>
+      </c>
+      <c r="G156" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>156</v>
+      </c>
+      <c r="B157" s="2">
+        <v>3</v>
+      </c>
+      <c r="C157" s="2">
+        <v>3</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F157" s="4">
+        <v>10</v>
+      </c>
+      <c r="G157" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H157" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>157</v>
+      </c>
+      <c r="B158" s="2">
+        <v>3</v>
+      </c>
+      <c r="C158" s="2">
+        <v>3</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F158" s="4">
+        <v>10</v>
+      </c>
+      <c r="G158" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H158" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>158</v>
+      </c>
+      <c r="B159" s="2">
+        <v>3</v>
+      </c>
+      <c r="C159" s="2">
+        <v>3</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F159" s="4">
+        <v>10</v>
+      </c>
+      <c r="G159" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H159" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>159</v>
+      </c>
+      <c r="B160" s="2">
+        <v>3</v>
+      </c>
+      <c r="C160" s="2">
+        <v>3</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F160" s="4">
+        <v>10</v>
+      </c>
+      <c r="G160" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>160</v>
+      </c>
+      <c r="B161" s="2">
+        <v>3</v>
+      </c>
+      <c r="C161" s="2">
+        <v>3</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F161" s="4">
+        <v>10</v>
+      </c>
+      <c r="G161" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="H161" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>161</v>
+      </c>
+      <c r="B162" s="2">
+        <v>3</v>
+      </c>
+      <c r="C162" s="2">
+        <v>2</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F162" s="4">
+        <v>6</v>
+      </c>
+      <c r="G162" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H162" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>162</v>
+      </c>
+      <c r="B163" s="2">
+        <v>3</v>
+      </c>
+      <c r="C163" s="2">
+        <v>2</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F163" s="4">
+        <v>6</v>
+      </c>
+      <c r="G163" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H163" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>163</v>
+      </c>
+      <c r="B164" s="2">
+        <v>3</v>
+      </c>
+      <c r="C164" s="2">
+        <v>2</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F164" s="4">
+        <v>6</v>
+      </c>
+      <c r="G164" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>164</v>
+      </c>
+      <c r="B165" s="2">
+        <v>3</v>
+      </c>
+      <c r="C165" s="2">
+        <v>2</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F165" s="4">
+        <v>6</v>
+      </c>
+      <c r="G165" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H165" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>165</v>
+      </c>
+      <c r="B166" s="2">
+        <v>3</v>
+      </c>
+      <c r="C166" s="2">
+        <v>2</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F166" s="4">
+        <v>6</v>
+      </c>
+      <c r="G166" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H166" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>166</v>
+      </c>
+      <c r="B167" s="2">
+        <v>3</v>
+      </c>
+      <c r="C167" s="2">
+        <v>2</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F167" s="4">
+        <v>6</v>
+      </c>
+      <c r="G167" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H167" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>167</v>
+      </c>
+      <c r="B168" s="2">
+        <v>3</v>
+      </c>
+      <c r="C168" s="2">
+        <v>2</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F168" s="4">
+        <v>6</v>
+      </c>
+      <c r="G168" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H168" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>168</v>
+      </c>
+      <c r="B169" s="2">
+        <v>3</v>
+      </c>
+      <c r="C169" s="2">
+        <v>2</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F169" s="4">
+        <v>6</v>
+      </c>
+      <c r="G169" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H169" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>169</v>
+      </c>
+      <c r="B170" s="2">
+        <v>3</v>
+      </c>
+      <c r="C170" s="2">
+        <v>2</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F170" s="4">
+        <v>6</v>
+      </c>
+      <c r="G170" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H170" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>170</v>
+      </c>
+      <c r="B171" s="2">
+        <v>3</v>
+      </c>
+      <c r="C171" s="2">
+        <v>2</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F171" s="4">
+        <v>6</v>
+      </c>
+      <c r="G171" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>171</v>
+      </c>
+      <c r="B172" s="2">
+        <v>3</v>
+      </c>
+      <c r="C172" s="2">
+        <v>2</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F172" s="4">
+        <v>6</v>
+      </c>
+      <c r="G172" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H172" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>172</v>
+      </c>
+      <c r="B173" s="2">
+        <v>3</v>
+      </c>
+      <c r="C173" s="2">
+        <v>2</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F173" s="4">
+        <v>6</v>
+      </c>
+      <c r="G173" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H173" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>173</v>
+      </c>
+      <c r="B174" s="2">
+        <v>3</v>
+      </c>
+      <c r="C174" s="2">
+        <v>2</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F174" s="4">
+        <v>6</v>
+      </c>
+      <c r="G174" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H174" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>174</v>
+      </c>
+      <c r="B175" s="2">
+        <v>3</v>
+      </c>
+      <c r="C175" s="2">
+        <v>2</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F175" s="4">
+        <v>6</v>
+      </c>
+      <c r="G175" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H175" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>175</v>
+      </c>
+      <c r="B176" s="2">
+        <v>3</v>
+      </c>
+      <c r="C176" s="2">
+        <v>2</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F176" s="4">
+        <v>6</v>
+      </c>
+      <c r="G176" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H176" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>176</v>
+      </c>
+      <c r="B177" s="2">
+        <v>3</v>
+      </c>
+      <c r="C177" s="2">
+        <v>2</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F177" s="4">
+        <v>6</v>
+      </c>
+      <c r="G177" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H177" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>177</v>
+      </c>
+      <c r="B178" s="2">
+        <v>3</v>
+      </c>
+      <c r="C178" s="2">
+        <v>2</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F178" s="4">
+        <v>6</v>
+      </c>
+      <c r="G178" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H178" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>178</v>
+      </c>
+      <c r="B179" s="2">
+        <v>3</v>
+      </c>
+      <c r="C179" s="2">
+        <v>2</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F179" s="4">
+        <v>6</v>
+      </c>
+      <c r="G179" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H179" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>179</v>
+      </c>
+      <c r="B180" s="2">
+        <v>3</v>
+      </c>
+      <c r="C180" s="2">
+        <v>2</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F180" s="4">
+        <v>6</v>
+      </c>
+      <c r="G180" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H180" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>180</v>
+      </c>
+      <c r="B181" s="2">
+        <v>3</v>
+      </c>
+      <c r="C181" s="2">
+        <v>2</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F181" s="4">
+        <v>6</v>
+      </c>
+      <c r="G181" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H181" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>181</v>
+      </c>
+      <c r="B182" s="2">
+        <v>3</v>
+      </c>
+      <c r="C182" s="2">
+        <v>2</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F182" s="4">
+        <v>6</v>
+      </c>
+      <c r="G182" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H182" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>182</v>
+      </c>
+      <c r="B183" s="2">
+        <v>3</v>
+      </c>
+      <c r="C183" s="2">
+        <v>2</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F183" s="4">
+        <v>6</v>
+      </c>
+      <c r="G183" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H183" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>183</v>
+      </c>
+      <c r="B184" s="2">
+        <v>3</v>
+      </c>
+      <c r="C184" s="2">
+        <v>2</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F184" s="4">
+        <v>6</v>
+      </c>
+      <c r="G184" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H184" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>184</v>
+      </c>
+      <c r="B185" s="2">
+        <v>3</v>
+      </c>
+      <c r="C185" s="2">
+        <v>2</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F185" s="4">
+        <v>6</v>
+      </c>
+      <c r="G185" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H185" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>185</v>
+      </c>
+      <c r="B186" s="2">
+        <v>3</v>
+      </c>
+      <c r="C186" s="2">
+        <v>2</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F186" s="4">
+        <v>6</v>
+      </c>
+      <c r="G186" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H186" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>186</v>
+      </c>
+      <c r="B187" s="2">
+        <v>3</v>
+      </c>
+      <c r="C187" s="2">
+        <v>2</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F187" s="4">
+        <v>6</v>
+      </c>
+      <c r="G187" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H187" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>187</v>
+      </c>
+      <c r="B188" s="2">
+        <v>3</v>
+      </c>
+      <c r="C188" s="2">
+        <v>2</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F188" s="4">
+        <v>6</v>
+      </c>
+      <c r="G188" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H188" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>188</v>
+      </c>
+      <c r="B189" s="2">
+        <v>3</v>
+      </c>
+      <c r="C189" s="2">
+        <v>2</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F189" s="4">
+        <v>6</v>
+      </c>
+      <c r="G189" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="H189" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>189</v>
+      </c>
+      <c r="B190" s="2">
+        <v>3</v>
+      </c>
+      <c r="C190" s="2">
+        <v>1</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F190" s="4">
+        <v>6</v>
+      </c>
+      <c r="G190" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H190" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>190</v>
+      </c>
+      <c r="B191" s="2">
+        <v>3</v>
+      </c>
+      <c r="C191" s="2">
+        <v>1</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F191" s="4">
+        <v>6</v>
+      </c>
+      <c r="G191" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H191" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>191</v>
+      </c>
+      <c r="B192" s="2">
+        <v>3</v>
+      </c>
+      <c r="C192" s="2">
+        <v>1</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F192" s="4">
+        <v>6</v>
+      </c>
+      <c r="G192" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H192" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>192</v>
+      </c>
+      <c r="B193" s="2">
+        <v>3</v>
+      </c>
+      <c r="C193" s="2">
+        <v>1</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F193" s="4">
+        <v>6</v>
+      </c>
+      <c r="G193" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H193" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>193</v>
+      </c>
+      <c r="B194" s="2">
+        <v>3</v>
+      </c>
+      <c r="C194" s="2">
+        <v>1</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F194" s="4">
+        <v>6</v>
+      </c>
+      <c r="G194" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H194" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>194</v>
+      </c>
+      <c r="B195" s="2">
+        <v>3</v>
+      </c>
+      <c r="C195" s="2">
+        <v>1</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F195" s="4">
+        <v>6</v>
+      </c>
+      <c r="G195" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H195" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>195</v>
+      </c>
+      <c r="B196" s="2">
+        <v>3</v>
+      </c>
+      <c r="C196" s="2">
+        <v>1</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F196" s="4">
+        <v>6</v>
+      </c>
+      <c r="G196" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H196" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>196</v>
+      </c>
+      <c r="B197" s="2">
+        <v>3</v>
+      </c>
+      <c r="C197" s="2">
+        <v>1</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F197" s="4">
+        <v>6</v>
+      </c>
+      <c r="G197" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H197" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>197</v>
+      </c>
+      <c r="B198" s="2">
+        <v>3</v>
+      </c>
+      <c r="C198" s="2">
+        <v>1</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F198" s="4">
+        <v>6</v>
+      </c>
+      <c r="G198" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H198" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>198</v>
+      </c>
+      <c r="B199" s="2">
+        <v>3</v>
+      </c>
+      <c r="C199" s="2">
+        <v>1</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F199" s="4">
+        <v>6</v>
+      </c>
+      <c r="G199" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H199" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>199</v>
+      </c>
+      <c r="B200" s="2">
+        <v>3</v>
+      </c>
+      <c r="C200" s="2">
+        <v>1</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F200" s="4">
+        <v>6</v>
+      </c>
+      <c r="G200" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H200" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>200</v>
+      </c>
+      <c r="B201" s="2">
+        <v>3</v>
+      </c>
+      <c r="C201" s="2">
+        <v>1</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F201" s="4">
+        <v>6</v>
+      </c>
+      <c r="G201" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H201" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>201</v>
+      </c>
+      <c r="B202" s="2">
+        <v>3</v>
+      </c>
+      <c r="C202" s="2">
+        <v>1</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F202" s="4">
+        <v>6</v>
+      </c>
+      <c r="G202" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H202" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>202</v>
+      </c>
+      <c r="B203" s="2">
+        <v>3</v>
+      </c>
+      <c r="C203" s="2">
+        <v>1</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F203" s="4">
+        <v>6</v>
+      </c>
+      <c r="G203" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H203" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>203</v>
+      </c>
+      <c r="B204" s="2">
+        <v>3</v>
+      </c>
+      <c r="C204" s="2">
+        <v>1</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F204" s="4">
+        <v>6</v>
+      </c>
+      <c r="G204" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H204" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>204</v>
+      </c>
+      <c r="B205" s="2">
+        <v>3</v>
+      </c>
+      <c r="C205" s="2">
+        <v>1</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F205" s="4">
+        <v>6</v>
+      </c>
+      <c r="G205" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H205" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>205</v>
+      </c>
+      <c r="B206" s="2">
+        <v>3</v>
+      </c>
+      <c r="C206" s="2">
+        <v>1</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F206" s="4">
+        <v>6</v>
+      </c>
+      <c r="G206" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H206" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>206</v>
+      </c>
+      <c r="B207" s="2">
+        <v>3</v>
+      </c>
+      <c r="C207" s="2">
+        <v>1</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F207" s="4">
+        <v>6</v>
+      </c>
+      <c r="G207" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H207" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>207</v>
+      </c>
+      <c r="B208" s="2">
+        <v>3</v>
+      </c>
+      <c r="C208" s="2">
+        <v>1</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F208" s="4">
+        <v>6</v>
+      </c>
+      <c r="G208" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H208" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>208</v>
+      </c>
+      <c r="B209" s="2">
+        <v>3</v>
+      </c>
+      <c r="C209" s="2">
+        <v>1</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F209" s="4">
+        <v>6</v>
+      </c>
+      <c r="G209" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H209" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>209</v>
+      </c>
+      <c r="B210" s="2">
+        <v>3</v>
+      </c>
+      <c r="C210" s="2">
+        <v>1</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F210" s="4">
+        <v>6</v>
+      </c>
+      <c r="G210" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H210" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>210</v>
+      </c>
+      <c r="B211" s="2">
+        <v>3</v>
+      </c>
+      <c r="C211" s="2">
+        <v>1</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F211" s="4">
+        <v>6</v>
+      </c>
+      <c r="G211" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H211" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>211</v>
+      </c>
+      <c r="B212" s="2">
+        <v>3</v>
+      </c>
+      <c r="C212" s="2">
+        <v>1</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F212" s="4">
+        <v>6</v>
+      </c>
+      <c r="G212" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H212" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>212</v>
+      </c>
+      <c r="B213" s="2">
+        <v>3</v>
+      </c>
+      <c r="C213" s="2">
+        <v>1</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F213" s="4">
+        <v>6</v>
+      </c>
+      <c r="G213" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H213" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>213</v>
+      </c>
+      <c r="B214" s="2">
+        <v>3</v>
+      </c>
+      <c r="C214" s="2">
+        <v>1</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F214" s="4">
+        <v>6</v>
+      </c>
+      <c r="G214" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H214" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>214</v>
+      </c>
+      <c r="B215" s="2">
+        <v>3</v>
+      </c>
+      <c r="C215" s="2">
+        <v>1</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F215" s="4">
+        <v>6</v>
+      </c>
+      <c r="G215" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H215" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>215</v>
+      </c>
+      <c r="B216" s="2">
+        <v>3</v>
+      </c>
+      <c r="C216" s="2">
+        <v>1</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F216" s="4">
+        <v>6</v>
+      </c>
+      <c r="G216" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H216" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>216</v>
+      </c>
+      <c r="B217" s="2">
+        <v>3</v>
+      </c>
+      <c r="C217" s="2">
+        <v>1</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F217" s="4">
+        <v>6</v>
+      </c>
+      <c r="G217" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H217" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>217</v>
+      </c>
+      <c r="B218" s="2">
+        <v>3</v>
+      </c>
+      <c r="C218" s="2">
+        <v>1</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F218" s="4">
+        <v>6</v>
+      </c>
+      <c r="G218" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H218" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>218</v>
+      </c>
+      <c r="B219" s="2">
+        <v>3</v>
+      </c>
+      <c r="C219" s="2">
+        <v>1</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F219" s="4">
+        <v>6</v>
+      </c>
+      <c r="G219" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H219" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>219</v>
+      </c>
+      <c r="B220" s="2">
+        <v>3</v>
+      </c>
+      <c r="C220" s="2">
+        <v>1</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F220" s="4">
+        <v>6</v>
+      </c>
+      <c r="G220" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H220" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>220</v>
+      </c>
+      <c r="B221" s="2">
+        <v>3</v>
+      </c>
+      <c r="C221" s="2">
+        <v>1</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F221" s="4">
+        <v>6</v>
+      </c>
+      <c r="G221" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H221" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>221</v>
+      </c>
+      <c r="B222" s="2">
+        <v>3</v>
+      </c>
+      <c r="C222" s="2">
+        <v>1</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F222" s="4">
+        <v>6</v>
+      </c>
+      <c r="G222" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H222" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>222</v>
+      </c>
+      <c r="B223" s="2">
+        <v>3</v>
+      </c>
+      <c r="C223" s="2">
+        <v>1</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F223" s="4">
+        <v>6</v>
+      </c>
+      <c r="G223" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="H223" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>223</v>
+      </c>
+      <c r="B224" s="2">
+        <v>3</v>
+      </c>
+      <c r="C224" s="2">
+        <v>2</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F224" s="4">
+        <v>4</v>
+      </c>
+      <c r="G224" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H224" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>224</v>
+      </c>
+      <c r="B225" s="2">
+        <v>3</v>
+      </c>
+      <c r="C225" s="2">
+        <v>2</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F225" s="4">
+        <v>4</v>
+      </c>
+      <c r="G225" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H225" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>225</v>
+      </c>
+      <c r="B226" s="2">
+        <v>3</v>
+      </c>
+      <c r="C226" s="2">
+        <v>2</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F226" s="4">
+        <v>4</v>
+      </c>
+      <c r="G226" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H226" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>226</v>
+      </c>
+      <c r="B227" s="2">
+        <v>3</v>
+      </c>
+      <c r="C227" s="2">
+        <v>2</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F227" s="4">
+        <v>4</v>
+      </c>
+      <c r="G227" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H227" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>227</v>
+      </c>
+      <c r="B228" s="2">
+        <v>3</v>
+      </c>
+      <c r="C228" s="2">
+        <v>2</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F228" s="4">
+        <v>4</v>
+      </c>
+      <c r="G228" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H228" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>228</v>
+      </c>
+      <c r="B229" s="2">
+        <v>3</v>
+      </c>
+      <c r="C229" s="2">
+        <v>2</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F229" s="4">
+        <v>4</v>
+      </c>
+      <c r="G229" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H229" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>229</v>
+      </c>
+      <c r="B230" s="2">
+        <v>3</v>
+      </c>
+      <c r="C230" s="2">
+        <v>2</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F230" s="4">
+        <v>4</v>
+      </c>
+      <c r="G230" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H230" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>230</v>
+      </c>
+      <c r="B231" s="2">
+        <v>3</v>
+      </c>
+      <c r="C231" s="2">
+        <v>2</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F231" s="4">
+        <v>4</v>
+      </c>
+      <c r="G231" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H231" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>231</v>
+      </c>
+      <c r="B232" s="2">
+        <v>3</v>
+      </c>
+      <c r="C232" s="2">
+        <v>2</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F232" s="4">
+        <v>4</v>
+      </c>
+      <c r="G232" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H232" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A233" s="2">
+        <v>232</v>
+      </c>
+      <c r="B233" s="2">
+        <v>3</v>
+      </c>
+      <c r="C233" s="2">
+        <v>2</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F233" s="4">
+        <v>4</v>
+      </c>
+      <c r="G233" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H233" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>233</v>
+      </c>
+      <c r="B234" s="2">
+        <v>3</v>
+      </c>
+      <c r="C234" s="2">
+        <v>2</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F234" s="4">
+        <v>4</v>
+      </c>
+      <c r="G234" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H234" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
+        <v>234</v>
+      </c>
+      <c r="B235" s="2">
+        <v>3</v>
+      </c>
+      <c r="C235" s="2">
+        <v>2</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F235" s="4">
+        <v>4</v>
+      </c>
+      <c r="G235" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H235" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A236" s="2">
+        <v>235</v>
+      </c>
+      <c r="B236" s="2">
+        <v>3</v>
+      </c>
+      <c r="C236" s="2">
+        <v>2</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F236" s="4">
+        <v>4</v>
+      </c>
+      <c r="G236" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H236" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A237" s="2">
+        <v>236</v>
+      </c>
+      <c r="B237" s="2">
+        <v>3</v>
+      </c>
+      <c r="C237" s="2">
+        <v>2</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F237" s="4">
+        <v>4</v>
+      </c>
+      <c r="G237" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H237" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
+        <v>237</v>
+      </c>
+      <c r="B238" s="2">
+        <v>3</v>
+      </c>
+      <c r="C238" s="2">
+        <v>2</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F238" s="4">
+        <v>4</v>
+      </c>
+      <c r="G238" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H238" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A239" s="2">
+        <v>238</v>
+      </c>
+      <c r="B239" s="2">
+        <v>3</v>
+      </c>
+      <c r="C239" s="2">
+        <v>2</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F239" s="4">
+        <v>4</v>
+      </c>
+      <c r="G239" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H239" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>239</v>
+      </c>
+      <c r="B240" s="2">
+        <v>3</v>
+      </c>
+      <c r="C240" s="2">
+        <v>2</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F240" s="4">
+        <v>4</v>
+      </c>
+      <c r="G240" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H240" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A241" s="2">
+        <v>240</v>
+      </c>
+      <c r="B241" s="2">
+        <v>3</v>
+      </c>
+      <c r="C241" s="2">
+        <v>2</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F241" s="4">
+        <v>4</v>
+      </c>
+      <c r="G241" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H241" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A242" s="2">
+        <v>241</v>
+      </c>
+      <c r="B242" s="2">
+        <v>3</v>
+      </c>
+      <c r="C242" s="2">
+        <v>2</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E242" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F242" s="4">
+        <v>4</v>
+      </c>
+      <c r="G242" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H242" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A243" s="2">
+        <v>242</v>
+      </c>
+      <c r="B243" s="2">
+        <v>3</v>
+      </c>
+      <c r="C243" s="2">
+        <v>2</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="F243" s="4">
+        <v>4</v>
+      </c>
+      <c r="G243" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H243" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A244" s="2">
+        <v>243</v>
+      </c>
+      <c r="B244" s="2">
+        <v>3</v>
+      </c>
+      <c r="C244" s="2">
+        <v>2</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F244" s="4">
+        <v>4</v>
+      </c>
+      <c r="G244" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H244" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A245" s="2">
+        <v>244</v>
+      </c>
+      <c r="B245" s="2">
+        <v>3</v>
+      </c>
+      <c r="C245" s="2">
+        <v>2</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E245" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F245" s="4">
+        <v>4</v>
+      </c>
+      <c r="G245" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H245" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>245</v>
+      </c>
+      <c r="B246" s="2">
+        <v>3</v>
+      </c>
+      <c r="C246" s="2">
+        <v>2</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="E246" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F246" s="4">
+        <v>4</v>
+      </c>
+      <c r="G246" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H246" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>246</v>
+      </c>
+      <c r="B247" s="2">
+        <v>3</v>
+      </c>
+      <c r="C247" s="2">
+        <v>2</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F247" s="4">
+        <v>4</v>
+      </c>
+      <c r="G247" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H247" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>247</v>
+      </c>
+      <c r="B248" s="2">
+        <v>3</v>
+      </c>
+      <c r="C248" s="2">
+        <v>2</v>
+      </c>
+      <c r="D248" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F248" s="4">
+        <v>4</v>
+      </c>
+      <c r="G248" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H248" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A249" s="2">
+        <v>248</v>
+      </c>
+      <c r="B249" s="2">
+        <v>3</v>
+      </c>
+      <c r="C249" s="2">
+        <v>2</v>
+      </c>
+      <c r="D249" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="E249" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F249" s="4">
+        <v>4</v>
+      </c>
+      <c r="G249" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H249" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>249</v>
+      </c>
+      <c r="B250" s="2">
+        <v>3</v>
+      </c>
+      <c r="C250" s="2">
+        <v>2</v>
+      </c>
+      <c r="D250" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="E250" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F250" s="4">
+        <v>4</v>
+      </c>
+      <c r="G250" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H250" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>250</v>
+      </c>
+      <c r="B251" s="2">
+        <v>3</v>
+      </c>
+      <c r="C251" s="2">
+        <v>2</v>
+      </c>
+      <c r="D251" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="E251" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F251" s="4">
+        <v>4</v>
+      </c>
+      <c r="G251" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H251" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>